<commit_message>
Update TestPlan - minor changes
</commit_message>
<xml_diff>
--- a/docs/StudyGroup_TestPlan.xlsx
+++ b/docs/StudyGroup_TestPlan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sergiistupkin/Downloads/study-group-feature/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sergiistupkin/study-group-feature/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4251097F-BD75-B740-AE4D-EE6EC81D63AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A55F7258-74DB-D54B-B528-37586AD8DA68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="760" windowWidth="31200" windowHeight="19920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="71">
-  <si>
-    <t>Title</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="72">
   <si>
     <t>Steps</t>
   </si>
@@ -118,45 +115,6 @@
     <t>Check invalid subject</t>
   </si>
   <si>
-    <t>Call CreateStudyGroup with valid name &amp; subject</t>
-  </si>
-  <si>
-    <t>Try to create group with 4-char name</t>
-  </si>
-  <si>
-    <t>Try with 31-char name</t>
-  </si>
-  <si>
-    <t>Same user creates 2 Math groups</t>
-  </si>
-  <si>
-    <t>Create one per subject</t>
-  </si>
-  <si>
-    <t>Call JoinStudyGroup</t>
-  </si>
-  <si>
-    <t>Call LeaveStudyGroup</t>
-  </si>
-  <si>
-    <t>Call GetStudyGroups</t>
-  </si>
-  <si>
-    <t>SearchStudyGroups('Math')</t>
-  </si>
-  <si>
-    <t>Fetch all groups sorted desc</t>
-  </si>
-  <si>
-    <t>Fetch all groups sorted asc</t>
-  </si>
-  <si>
-    <t>Create group then join</t>
-  </si>
-  <si>
-    <t>Try to create with invalid subject</t>
-  </si>
-  <si>
     <t>Name: 'Math Wizards', Subject: Math</t>
   </si>
   <si>
@@ -233,6 +191,73 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>TC Title</t>
+  </si>
+  <si>
+    <t>1. Prepare a valid StudyGroup object with name 'Math Wizards' and subject 'Math'
+2. Call the CreateStudyGroup API
+3. Verify response is successful</t>
+  </si>
+  <si>
+    <t>1. Prepare a StudyGroup object with a 4-character name
+2. Call the CreateStudyGroup API or constructor
+3. Validate that a name length validation error is returned</t>
+  </si>
+  <si>
+    <t>1. Prepare a StudyGroup object with a 31-character name
+2. Call the CreateStudyGroup API or constructor
+3. Validate that a name length validation error is returned</t>
+  </si>
+  <si>
+    <t>1. User creates a StudyGroup for subject 'Math'
+2. Attempt to create a second group for 'Math' by the same user
+3. Verify that second creation is rejected</t>
+  </si>
+  <si>
+    <t>1. Create separate StudyGroups for 'Math', 'Physics', 'Chemistry'
+2. Verify all are created successfully without conflict</t>
+  </si>
+  <si>
+    <t>1. Choose an existing StudyGroup
+2. Call JoinStudyGroup API with GroupId and UserId
+3. Verify user is added to the group</t>
+  </si>
+  <si>
+    <t>1. Choose a StudyGroup that the user has joined
+2. Call LeaveStudyGroup API
+3. Verify user is removed from the group</t>
+  </si>
+  <si>
+    <t>1. Call GetStudyGroups API
+2. Verify that all groups are returned in the response</t>
+  </si>
+  <si>
+    <t>1. Call SearchStudyGroups API with subject = 'Math'
+2. Verify that only groups with Math subject are returned</t>
+  </si>
+  <si>
+    <t>1. Use the app UI to open the StudyGroups list
+2. Apply 'sort by newest' option
+3. Verify groups are sorted by descending creation date</t>
+  </si>
+  <si>
+    <t>1. Use the app UI to open the StudyGroups list
+2. Apply 'sort by oldest' option
+3. Verify groups are sorted by ascending creation date</t>
+  </si>
+  <si>
+    <t>1. User creates a StudyGroup
+2. Same user joins the created group
+3. Verify join operation is successful</t>
+  </si>
+  <si>
+    <t>1. Attempt to create a StudyGroup with subject 'Biology'
+2. Verify that the request is rejected with invalid subject error</t>
   </si>
 </sst>
 </file>
@@ -621,7 +646,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -637,323 +662,325 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A1" s="3"/>
+      <c r="A1" s="3" t="s">
+        <v>57</v>
+      </c>
       <c r="B1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="B2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C3" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="119" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="111" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F7" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="G2" s="5" t="s">
+      <c r="G11" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="4" t="s">
+      <c r="D13" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="E13" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="4" t="s">
+      <c r="F13" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="E14" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" s="4" t="s">
+      <c r="F14" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E14" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>68</v>
-      </c>
       <c r="G14" s="5" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added unit and component test cases, added one test case to Test Plan, updated Readme
</commit_message>
<xml_diff>
--- a/docs/StudyGroup_TestPlan.xlsx
+++ b/docs/StudyGroup_TestPlan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10402"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sergiistupkin/study-group-feature/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A55F7258-74DB-D54B-B528-37586AD8DA68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AF6FE86-1BA0-4F4E-80A8-527046283B1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="760" windowWidth="31200" windowHeight="19920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="77">
   <si>
     <t>Steps</t>
   </si>
@@ -258,6 +258,23 @@
   <si>
     <t>1. Attempt to create a StudyGroup with subject 'Biology'
 2. Verify that the request is rejected with invalid subject error</t>
+  </si>
+  <si>
+    <t>TC14</t>
+  </si>
+  <si>
+    <t>1. Create a StudyGroup object with name 'Physics Stars' and Subject.Physics
+2. Ensure the object is initialized correctly
+3. Validate the name and subject fields</t>
+  </si>
+  <si>
+    <t>Name: 'Physics Stars', Subject: Physics</t>
+  </si>
+  <si>
+    <t>StudyGroup object is created with correct values</t>
+  </si>
+  <si>
+    <t>Check Valid subject</t>
   </si>
 </sst>
 </file>
@@ -643,10 +660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -960,26 +977,49 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="119" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>30</v>
+        <v>76</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>40</v>
+        <v>74</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="G14" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G15" s="5" t="s">
         <v>56</v>
       </c>
     </row>

</xml_diff>